<commit_message>
Genra arrays added, but now working on spaces
</commit_message>
<xml_diff>
--- a/ArrayInfo.xlsx
+++ b/ArrayInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="300" windowWidth="22692" windowHeight="9012" activeTab="1"/>
+    <workbookView xWindow="288" yWindow="300" windowWidth="22692" windowHeight="9012"/>
   </bookViews>
   <sheets>
     <sheet name="Music" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="386">
   <si>
     <t>Spot</t>
   </si>
@@ -757,6 +757,426 @@
   </si>
   <si>
     <t>Youngblood</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Top Gun", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Crocodile Dundee", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Platoon", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"The Karate Kid Part II", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Star Trek IV: The Voyage Home", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Back to School", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Aliens", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"The Golden Child", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Ruthless People", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Ferris Bueller's Day Off", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Down and Out in Beverly Hills", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"The Color of Money", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Stand by Me", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Legal Eagles", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Cobra", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"An American Tail", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Police Academy 3: Back in Training", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Heartbreak Ridge", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Peggy Sue Got Married", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Poltergeist II: The Other Side", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Short Circuit", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Pretty in Pink", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"The Fly", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Three Amigos", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Little Shop of Horrors", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"About Last Night...", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Running Scared", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"The Money Pit", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Gung Ho", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Hannah and Her Sisters", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Nothing in Common", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Children of a Lesser God", </t>
+  </si>
+  <si>
+    <t>43453Lady and the Tramp (re</t>
+  </si>
+  <si>
+    <t>43425Song of the South (Re</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Glory of Love </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> There'll Be Sad Songs </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Don't Forget Me </t>
+  </si>
+  <si>
+    <t>" That's What Friends Are For ",</t>
+  </si>
+  <si>
+    <t>" Say You, Say Me ",</t>
+  </si>
+  <si>
+    <t>" I Miss You ",</t>
+  </si>
+  <si>
+    <t>" On My Own ",</t>
+  </si>
+  <si>
+    <t>" Broken Wings ",</t>
+  </si>
+  <si>
+    <t>" How Will I Know ",</t>
+  </si>
+  <si>
+    <t>" Party All the Time ",</t>
+  </si>
+  <si>
+    <t>" Burning Heart ",</t>
+  </si>
+  <si>
+    <t>" Kyrie ",</t>
+  </si>
+  <si>
+    <t>" Addicted to Love ",</t>
+  </si>
+  <si>
+    <t>" Greatest Love of All ",</t>
+  </si>
+  <si>
+    <t>" Secret Lovers ",</t>
+  </si>
+  <si>
+    <t>" Friends &amp; Lovers ",</t>
+  </si>
+  <si>
+    <t>" Glory of Love ",</t>
+  </si>
+  <si>
+    <t>" West End Girls ",</t>
+  </si>
+  <si>
+    <t>" There'll Be Sad Songs ",</t>
+  </si>
+  <si>
+    <t>" Alive and Kicking ",</t>
+  </si>
+  <si>
+    <t>" Never ",</t>
+  </si>
+  <si>
+    <t>" Kiss ",</t>
+  </si>
+  <si>
+    <t>" Higher Love ",</t>
+  </si>
+  <si>
+    <t>" Stuck With You ",</t>
+  </si>
+  <si>
+    <t>" Holding Back the Years ",</t>
+  </si>
+  <si>
+    <t>" Sledgehammer ",</t>
+  </si>
+  <si>
+    <t>" Sara ",</t>
+  </si>
+  <si>
+    <t>" Human ",</t>
+  </si>
+  <si>
+    <t>" I Can't Wait ",</t>
+  </si>
+  <si>
+    <t>" Take My Breath Away ",</t>
+  </si>
+  <si>
+    <t>" Rock Me Amadeus ",</t>
+  </si>
+  <si>
+    <t>" Papa Don't Preach ",</t>
+  </si>
+  <si>
+    <t>" You Give Love a Bad Name ",</t>
+  </si>
+  <si>
+    <t>" When the Going Gets Tough, The Tough Get Going ",</t>
+  </si>
+  <si>
+    <t>" When I Think of You ",</t>
+  </si>
+  <si>
+    <t>" These Dreams ",</t>
+  </si>
+  <si>
+    <t>" Don't Forget Me ",</t>
+  </si>
+  <si>
+    <t>" Live to Tell ",</t>
+  </si>
+  <si>
+    <t>" Mad About You ",</t>
+  </si>
+  <si>
+    <t>" Something About You ",</t>
+  </si>
+  <si>
+    <t>" Venus ",</t>
+  </si>
+  <si>
+    <t>" Dancing On the Ceiling ",</t>
+  </si>
+  <si>
+    <t>" Conga ",</t>
+  </si>
+  <si>
+    <t>" True Colors ",</t>
+  </si>
+  <si>
+    <t>" Danger Zone ",</t>
+  </si>
+  <si>
+    <t>" What Have You Done for Me Lately ",</t>
+  </si>
+  <si>
+    <t>" No One Is to Blame ",</t>
+  </si>
+  <si>
+    <t>" Let's Go All the Way ",</t>
+  </si>
+  <si>
+    <t>" I Didn't Mean to Turn You On ",</t>
+  </si>
+  <si>
+    <t>" Words Get In the Way ",</t>
+  </si>
+  <si>
+    <t>" Manic Monday ",</t>
+  </si>
+  <si>
+    <t>" Walk of Life ",</t>
+  </si>
+  <si>
+    <t>" Amanda ",</t>
+  </si>
+  <si>
+    <t>" Two of Hearts ",</t>
+  </si>
+  <si>
+    <t>" Crush On You ",</t>
+  </si>
+  <si>
+    <t>" If You Leave ",</t>
+  </si>
+  <si>
+    <t>" Invisible Touch ",</t>
+  </si>
+  <si>
+    <t>" The Sweetest Taboo ",</t>
+  </si>
+  <si>
+    <t>" What You Need ",</t>
+  </si>
+  <si>
+    <t>" Talk to Me ",</t>
+  </si>
+  <si>
+    <t>" Nasty ",</t>
+  </si>
+  <si>
+    <t>" Take Me Home Tonight ",</t>
+  </si>
+  <si>
+    <t>" We Don't Have to Take Our Clothes Off ",</t>
+  </si>
+  <si>
+    <t>" All Cried Out ",</t>
+  </si>
+  <si>
+    <t>" Your Love ",</t>
+  </si>
+  <si>
+    <t>" I'm Your Man ",</t>
+  </si>
+  <si>
+    <t>" Perfect Way ",</t>
+  </si>
+  <si>
+    <t>" Living In America ",</t>
+  </si>
+  <si>
+    <t>" R O C K in the USA  ",</t>
+  </si>
+  <si>
+    <t>" Who's Johnny ",</t>
+  </si>
+  <si>
+    <t>" Word Up ",</t>
+  </si>
+  <si>
+    <t>" Why Can't This Be Love ",</t>
+  </si>
+  <si>
+    <t>" Silent Running ",</t>
+  </si>
+  <si>
+    <t>" Typical Male ",</t>
+  </si>
+  <si>
+    <t>" Small Town ",</t>
+  </si>
+  <si>
+    <t>" Tarzan Boy ",</t>
+  </si>
+  <si>
+    <t>" All I Need Is A Miracle ",</t>
+  </si>
+  <si>
+    <t>" Sweet Freedom ",</t>
+  </si>
+  <si>
+    <t>" True Blue ",</t>
+  </si>
+  <si>
+    <t>" Rumors, Timex Social Club",</t>
+  </si>
+  <si>
+    <t>" Life In a Northern Town ",</t>
+  </si>
+  <si>
+    <t>" Bad Boy ",</t>
+  </si>
+  <si>
+    <t>" Sleeping Bag ",</t>
+  </si>
+  <si>
+    <t>" Tonight She Comes ",</t>
+  </si>
+  <si>
+    <t>" Love Touch ",</t>
+  </si>
+  <si>
+    <t>" A Love Bizarre ",</t>
+  </si>
+  <si>
+    <t>" Throwing It All Away ",</t>
+  </si>
+  <si>
+    <t>" Baby Love ",</t>
+  </si>
+  <si>
+    <t>" Election Day ",</t>
+  </si>
+  <si>
+    <t>" Nikita ",</t>
+  </si>
+  <si>
+    <t>" Take Me Home ",</t>
+  </si>
+  <si>
+    <t>" Walk This Way ",</t>
+  </si>
+  <si>
+    <t>" Sweet Love ",</t>
+  </si>
+  <si>
+    <t>" Your Wildest Dreams ",</t>
+  </si>
+  <si>
+    <t>" Spies Like Us ",</t>
+  </si>
+  <si>
+    <t>" Object of My Desire ",</t>
+  </si>
+  <si>
+    <t>" Dreamtime ",</t>
+  </si>
+  <si>
+    <t>" Tender Love ",</t>
+  </si>
+  <si>
+    <t>" King for a Day ",</t>
+  </si>
+  <si>
+    <t>" Love Will Conquer All ",</t>
+  </si>
+  <si>
+    <t>" A Different Corner ",</t>
+  </si>
+  <si>
+    <t>" I'll Be Over You ",</t>
+  </si>
+  <si>
+    <t>" Go Home ",</t>
   </si>
 </sst>
 </file>
@@ -792,9 +1212,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1096,10 +1515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:DE101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1107,9 +1526,11 @@
     <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1119,8 +1540,311 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>286</v>
+      </c>
+      <c r="K1" t="s">
+        <v>287</v>
+      </c>
+      <c r="L1" t="s">
+        <v>288</v>
+      </c>
+      <c r="M1" t="s">
+        <v>289</v>
+      </c>
+      <c r="N1" t="s">
+        <v>290</v>
+      </c>
+      <c r="O1" t="s">
+        <v>291</v>
+      </c>
+      <c r="P1" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>293</v>
+      </c>
+      <c r="R1" t="s">
+        <v>294</v>
+      </c>
+      <c r="S1" t="s">
+        <v>295</v>
+      </c>
+      <c r="T1" t="s">
+        <v>296</v>
+      </c>
+      <c r="U1" t="s">
+        <v>297</v>
+      </c>
+      <c r="V1" t="s">
+        <v>298</v>
+      </c>
+      <c r="W1" t="s">
+        <v>299</v>
+      </c>
+      <c r="X1" t="s">
+        <v>300</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>301</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>302</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>304</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>305</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>306</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>307</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>308</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>309</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>311</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>312</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>313</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>314</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>315</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>316</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>317</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>318</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>319</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>320</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>323</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>324</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>326</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>327</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>328</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>329</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>330</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>331</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>332</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>333</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>334</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>335</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>336</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>337</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>338</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>339</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>340</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>341</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>342</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>343</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>344</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>345</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>346</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>347</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>348</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>349</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>350</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>351</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>352</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>354</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>355</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>356</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>357</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>358</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>359</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>360</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>361</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>362</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>363</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>364</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>365</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>366</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>368</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>369</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>370</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>371</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>372</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>373</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>374</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>375</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>376</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>377</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>378</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>379</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>380</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>381</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>382</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>383</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>384</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1130,8 +1854,23 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" t="s">
+        <v>246</v>
+      </c>
+      <c r="H2" t="s">
+        <v>247</v>
+      </c>
+      <c r="I2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1141,8 +1880,23 @@
       <c r="C3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H3" t="s">
+        <v>247</v>
+      </c>
+      <c r="I3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1152,8 +1906,23 @@
       <c r="C4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G4" t="s">
+        <v>246</v>
+      </c>
+      <c r="H4" t="s">
+        <v>247</v>
+      </c>
+      <c r="I4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1163,8 +1932,23 @@
       <c r="C5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
+        <v>246</v>
+      </c>
+      <c r="G5" t="s">
+        <v>246</v>
+      </c>
+      <c r="H5" t="s">
+        <v>247</v>
+      </c>
+      <c r="I5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1174,8 +1958,23 @@
       <c r="C6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" t="s">
+        <v>246</v>
+      </c>
+      <c r="G6" t="s">
+        <v>246</v>
+      </c>
+      <c r="H6" t="s">
+        <v>247</v>
+      </c>
+      <c r="I6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1185,8 +1984,23 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" t="s">
+        <v>246</v>
+      </c>
+      <c r="G7" t="s">
+        <v>246</v>
+      </c>
+      <c r="H7" t="s">
+        <v>247</v>
+      </c>
+      <c r="I7" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="8" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1196,8 +2010,23 @@
       <c r="C8" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" t="s">
+        <v>246</v>
+      </c>
+      <c r="G8" t="s">
+        <v>246</v>
+      </c>
+      <c r="H8" t="s">
+        <v>247</v>
+      </c>
+      <c r="I8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1207,8 +2036,23 @@
       <c r="C9" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F9" t="s">
+        <v>246</v>
+      </c>
+      <c r="G9" t="s">
+        <v>246</v>
+      </c>
+      <c r="H9" t="s">
+        <v>247</v>
+      </c>
+      <c r="I9" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1218,8 +2062,23 @@
       <c r="C10" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G10" t="s">
+        <v>246</v>
+      </c>
+      <c r="H10" t="s">
+        <v>247</v>
+      </c>
+      <c r="I10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1229,8 +2088,23 @@
       <c r="C11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>246</v>
+      </c>
+      <c r="G11" t="s">
+        <v>246</v>
+      </c>
+      <c r="H11" t="s">
+        <v>247</v>
+      </c>
+      <c r="I11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="12" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1240,8 +2114,23 @@
       <c r="C12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>246</v>
+      </c>
+      <c r="G12" t="s">
+        <v>246</v>
+      </c>
+      <c r="H12" t="s">
+        <v>247</v>
+      </c>
+      <c r="I12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1251,8 +2140,23 @@
       <c r="C13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>246</v>
+      </c>
+      <c r="G13" t="s">
+        <v>246</v>
+      </c>
+      <c r="H13" t="s">
+        <v>247</v>
+      </c>
+      <c r="I13" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="14" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1262,8 +2166,23 @@
       <c r="C14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>246</v>
+      </c>
+      <c r="G14" t="s">
+        <v>246</v>
+      </c>
+      <c r="H14" t="s">
+        <v>247</v>
+      </c>
+      <c r="I14" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="15" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1273,8 +2192,23 @@
       <c r="C15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>283</v>
+      </c>
+      <c r="F15" t="s">
+        <v>246</v>
+      </c>
+      <c r="G15" t="s">
+        <v>246</v>
+      </c>
+      <c r="H15" t="s">
+        <v>247</v>
+      </c>
+      <c r="I15" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="16" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1284,8 +2218,23 @@
       <c r="C16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>246</v>
+      </c>
+      <c r="G16" t="s">
+        <v>246</v>
+      </c>
+      <c r="H16" t="s">
+        <v>247</v>
+      </c>
+      <c r="I16" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1295,8 +2244,23 @@
       <c r="C17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>284</v>
+      </c>
+      <c r="F17" t="s">
+        <v>246</v>
+      </c>
+      <c r="G17" t="s">
+        <v>246</v>
+      </c>
+      <c r="H17" t="s">
+        <v>247</v>
+      </c>
+      <c r="I17" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1306,8 +2270,23 @@
       <c r="C18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>246</v>
+      </c>
+      <c r="G18" t="s">
+        <v>246</v>
+      </c>
+      <c r="H18" t="s">
+        <v>247</v>
+      </c>
+      <c r="I18" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1317,8 +2296,23 @@
       <c r="C19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" t="s">
+        <v>246</v>
+      </c>
+      <c r="G19" t="s">
+        <v>246</v>
+      </c>
+      <c r="H19" t="s">
+        <v>247</v>
+      </c>
+      <c r="I19" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1328,8 +2322,23 @@
       <c r="C20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>246</v>
+      </c>
+      <c r="G20" t="s">
+        <v>246</v>
+      </c>
+      <c r="H20" t="s">
+        <v>247</v>
+      </c>
+      <c r="I20" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1339,8 +2348,23 @@
       <c r="C21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" t="s">
+        <v>246</v>
+      </c>
+      <c r="G21" t="s">
+        <v>246</v>
+      </c>
+      <c r="H21" t="s">
+        <v>247</v>
+      </c>
+      <c r="I21" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1350,8 +2374,23 @@
       <c r="C22" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" t="s">
+        <v>246</v>
+      </c>
+      <c r="G22" t="s">
+        <v>246</v>
+      </c>
+      <c r="H22" t="s">
+        <v>247</v>
+      </c>
+      <c r="I22" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1361,8 +2400,23 @@
       <c r="C23" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" t="s">
+        <v>246</v>
+      </c>
+      <c r="G23" t="s">
+        <v>246</v>
+      </c>
+      <c r="H23" t="s">
+        <v>247</v>
+      </c>
+      <c r="I23" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1372,8 +2426,23 @@
       <c r="C24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>246</v>
+      </c>
+      <c r="G24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H24" t="s">
+        <v>247</v>
+      </c>
+      <c r="I24" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1383,8 +2452,23 @@
       <c r="C25" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" t="s">
+        <v>246</v>
+      </c>
+      <c r="G25" t="s">
+        <v>246</v>
+      </c>
+      <c r="H25" t="s">
+        <v>247</v>
+      </c>
+      <c r="I25" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1394,8 +2478,23 @@
       <c r="C26" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" t="s">
+        <v>246</v>
+      </c>
+      <c r="G26" t="s">
+        <v>246</v>
+      </c>
+      <c r="H26" t="s">
+        <v>247</v>
+      </c>
+      <c r="I26" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1405,8 +2504,23 @@
       <c r="C27" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" t="s">
+        <v>246</v>
+      </c>
+      <c r="G27" t="s">
+        <v>246</v>
+      </c>
+      <c r="H27" t="s">
+        <v>247</v>
+      </c>
+      <c r="I27" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1416,8 +2530,23 @@
       <c r="C28" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" t="s">
+        <v>246</v>
+      </c>
+      <c r="G28" t="s">
+        <v>246</v>
+      </c>
+      <c r="H28" t="s">
+        <v>247</v>
+      </c>
+      <c r="I28" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1427,8 +2556,23 @@
       <c r="C29" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" t="s">
+        <v>246</v>
+      </c>
+      <c r="G29" t="s">
+        <v>246</v>
+      </c>
+      <c r="H29" t="s">
+        <v>247</v>
+      </c>
+      <c r="I29" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1438,8 +2582,23 @@
       <c r="C30" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" t="s">
+        <v>246</v>
+      </c>
+      <c r="G30" t="s">
+        <v>246</v>
+      </c>
+      <c r="H30" t="s">
+        <v>247</v>
+      </c>
+      <c r="I30" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1449,8 +2608,23 @@
       <c r="C31" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" t="s">
+        <v>246</v>
+      </c>
+      <c r="G31" t="s">
+        <v>246</v>
+      </c>
+      <c r="H31" t="s">
+        <v>247</v>
+      </c>
+      <c r="I31" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1460,8 +2634,23 @@
       <c r="C32" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" t="s">
+        <v>246</v>
+      </c>
+      <c r="G32" t="s">
+        <v>246</v>
+      </c>
+      <c r="H32" t="s">
+        <v>247</v>
+      </c>
+      <c r="I32" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1471,8 +2660,23 @@
       <c r="C33" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" t="s">
+        <v>246</v>
+      </c>
+      <c r="G33" t="s">
+        <v>246</v>
+      </c>
+      <c r="H33" t="s">
+        <v>247</v>
+      </c>
+      <c r="I33" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1482,8 +2686,23 @@
       <c r="C34" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" t="s">
+        <v>246</v>
+      </c>
+      <c r="G34" t="s">
+        <v>246</v>
+      </c>
+      <c r="H34" t="s">
+        <v>247</v>
+      </c>
+      <c r="I34" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1493,8 +2712,23 @@
       <c r="C35" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>285</v>
+      </c>
+      <c r="F35" t="s">
+        <v>246</v>
+      </c>
+      <c r="G35" t="s">
+        <v>246</v>
+      </c>
+      <c r="H35" t="s">
+        <v>247</v>
+      </c>
+      <c r="I35" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1504,8 +2738,23 @@
       <c r="C36" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
+        <v>59</v>
+      </c>
+      <c r="F36" t="s">
+        <v>246</v>
+      </c>
+      <c r="G36" t="s">
+        <v>246</v>
+      </c>
+      <c r="H36" t="s">
+        <v>247</v>
+      </c>
+      <c r="I36" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1515,8 +2764,23 @@
       <c r="C37" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" t="s">
+        <v>246</v>
+      </c>
+      <c r="G37" t="s">
+        <v>246</v>
+      </c>
+      <c r="H37" t="s">
+        <v>247</v>
+      </c>
+      <c r="I37" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1526,8 +2790,23 @@
       <c r="C38" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" t="s">
+        <v>246</v>
+      </c>
+      <c r="G38" t="s">
+        <v>246</v>
+      </c>
+      <c r="H38" t="s">
+        <v>247</v>
+      </c>
+      <c r="I38" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1537,8 +2816,23 @@
       <c r="C39" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" t="s">
+        <v>246</v>
+      </c>
+      <c r="G39" t="s">
+        <v>246</v>
+      </c>
+      <c r="H39" t="s">
+        <v>247</v>
+      </c>
+      <c r="I39" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1548,8 +2842,23 @@
       <c r="C40" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>66</v>
+      </c>
+      <c r="F40" t="s">
+        <v>246</v>
+      </c>
+      <c r="G40" t="s">
+        <v>246</v>
+      </c>
+      <c r="H40" t="s">
+        <v>247</v>
+      </c>
+      <c r="I40" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1559,8 +2868,23 @@
       <c r="C41" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" t="s">
+        <v>246</v>
+      </c>
+      <c r="G41" t="s">
+        <v>246</v>
+      </c>
+      <c r="H41" t="s">
+        <v>247</v>
+      </c>
+      <c r="I41" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1570,8 +2894,23 @@
       <c r="C42" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" t="s">
+        <v>246</v>
+      </c>
+      <c r="G42" t="s">
+        <v>246</v>
+      </c>
+      <c r="H42" t="s">
+        <v>247</v>
+      </c>
+      <c r="I42" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1581,8 +2920,23 @@
       <c r="C43" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43" t="s">
+        <v>246</v>
+      </c>
+      <c r="G43" t="s">
+        <v>246</v>
+      </c>
+      <c r="H43" t="s">
+        <v>247</v>
+      </c>
+      <c r="I43" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1592,8 +2946,23 @@
       <c r="C44" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>75</v>
+      </c>
+      <c r="F44" t="s">
+        <v>246</v>
+      </c>
+      <c r="G44" t="s">
+        <v>246</v>
+      </c>
+      <c r="H44" t="s">
+        <v>247</v>
+      </c>
+      <c r="I44" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1603,8 +2972,23 @@
       <c r="C45" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E45" t="s">
+        <v>76</v>
+      </c>
+      <c r="F45" t="s">
+        <v>246</v>
+      </c>
+      <c r="G45" t="s">
+        <v>246</v>
+      </c>
+      <c r="H45" t="s">
+        <v>247</v>
+      </c>
+      <c r="I45" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1614,8 +2998,23 @@
       <c r="C46" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E46" t="s">
+        <v>78</v>
+      </c>
+      <c r="F46" t="s">
+        <v>246</v>
+      </c>
+      <c r="G46" t="s">
+        <v>246</v>
+      </c>
+      <c r="H46" t="s">
+        <v>247</v>
+      </c>
+      <c r="I46" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1625,8 +3024,23 @@
       <c r="C47" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E47" t="s">
+        <v>80</v>
+      </c>
+      <c r="F47" t="s">
+        <v>246</v>
+      </c>
+      <c r="G47" t="s">
+        <v>246</v>
+      </c>
+      <c r="H47" t="s">
+        <v>247</v>
+      </c>
+      <c r="I47" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1636,8 +3050,23 @@
       <c r="C48" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>81</v>
+      </c>
+      <c r="F48" t="s">
+        <v>246</v>
+      </c>
+      <c r="G48" t="s">
+        <v>246</v>
+      </c>
+      <c r="H48" t="s">
+        <v>247</v>
+      </c>
+      <c r="I48" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1647,8 +3076,23 @@
       <c r="C49" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E49" t="s">
+        <v>82</v>
+      </c>
+      <c r="F49" t="s">
+        <v>246</v>
+      </c>
+      <c r="G49" t="s">
+        <v>246</v>
+      </c>
+      <c r="H49" t="s">
+        <v>247</v>
+      </c>
+      <c r="I49" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1658,8 +3102,23 @@
       <c r="C50" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E50" t="s">
+        <v>84</v>
+      </c>
+      <c r="F50" t="s">
+        <v>246</v>
+      </c>
+      <c r="G50" t="s">
+        <v>246</v>
+      </c>
+      <c r="H50" t="s">
+        <v>247</v>
+      </c>
+      <c r="I50" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1669,8 +3128,23 @@
       <c r="C51" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E51" t="s">
+        <v>88</v>
+      </c>
+      <c r="F51" t="s">
+        <v>246</v>
+      </c>
+      <c r="G51" t="s">
+        <v>246</v>
+      </c>
+      <c r="H51" t="s">
+        <v>247</v>
+      </c>
+      <c r="I51" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1680,8 +3154,23 @@
       <c r="C52" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E52" t="s">
+        <v>90</v>
+      </c>
+      <c r="F52" t="s">
+        <v>246</v>
+      </c>
+      <c r="G52" t="s">
+        <v>246</v>
+      </c>
+      <c r="H52" t="s">
+        <v>247</v>
+      </c>
+      <c r="I52" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1691,8 +3180,23 @@
       <c r="C53" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E53" t="s">
+        <v>92</v>
+      </c>
+      <c r="F53" t="s">
+        <v>246</v>
+      </c>
+      <c r="G53" t="s">
+        <v>246</v>
+      </c>
+      <c r="H53" t="s">
+        <v>247</v>
+      </c>
+      <c r="I53" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1702,8 +3206,23 @@
       <c r="C54" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E54" t="s">
+        <v>94</v>
+      </c>
+      <c r="F54" t="s">
+        <v>246</v>
+      </c>
+      <c r="G54" t="s">
+        <v>246</v>
+      </c>
+      <c r="H54" t="s">
+        <v>247</v>
+      </c>
+      <c r="I54" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1713,8 +3232,23 @@
       <c r="C55" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E55" t="s">
+        <v>96</v>
+      </c>
+      <c r="F55" t="s">
+        <v>246</v>
+      </c>
+      <c r="G55" t="s">
+        <v>246</v>
+      </c>
+      <c r="H55" t="s">
+        <v>247</v>
+      </c>
+      <c r="I55" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1724,8 +3258,23 @@
       <c r="C56" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E56" t="s">
+        <v>98</v>
+      </c>
+      <c r="F56" t="s">
+        <v>246</v>
+      </c>
+      <c r="G56" t="s">
+        <v>246</v>
+      </c>
+      <c r="H56" t="s">
+        <v>247</v>
+      </c>
+      <c r="I56" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1735,8 +3284,23 @@
       <c r="C57" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E57" t="s">
+        <v>100</v>
+      </c>
+      <c r="F57" t="s">
+        <v>246</v>
+      </c>
+      <c r="G57" t="s">
+        <v>246</v>
+      </c>
+      <c r="H57" t="s">
+        <v>247</v>
+      </c>
+      <c r="I57" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1746,8 +3310,23 @@
       <c r="C58" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E58" t="s">
+        <v>102</v>
+      </c>
+      <c r="F58" t="s">
+        <v>246</v>
+      </c>
+      <c r="G58" t="s">
+        <v>246</v>
+      </c>
+      <c r="H58" t="s">
+        <v>247</v>
+      </c>
+      <c r="I58" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1757,8 +3336,23 @@
       <c r="C59" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E59" t="s">
+        <v>104</v>
+      </c>
+      <c r="F59" t="s">
+        <v>246</v>
+      </c>
+      <c r="G59" t="s">
+        <v>246</v>
+      </c>
+      <c r="H59" t="s">
+        <v>247</v>
+      </c>
+      <c r="I59" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1768,8 +3362,23 @@
       <c r="C60" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E60" t="s">
+        <v>105</v>
+      </c>
+      <c r="F60" t="s">
+        <v>246</v>
+      </c>
+      <c r="G60" t="s">
+        <v>246</v>
+      </c>
+      <c r="H60" t="s">
+        <v>247</v>
+      </c>
+      <c r="I60" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1779,8 +3388,23 @@
       <c r="C61" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E61" t="s">
+        <v>108</v>
+      </c>
+      <c r="F61" t="s">
+        <v>246</v>
+      </c>
+      <c r="G61" t="s">
+        <v>246</v>
+      </c>
+      <c r="H61" t="s">
+        <v>247</v>
+      </c>
+      <c r="I61" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1790,8 +3414,23 @@
       <c r="C62" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E62" t="s">
+        <v>110</v>
+      </c>
+      <c r="F62" t="s">
+        <v>246</v>
+      </c>
+      <c r="G62" t="s">
+        <v>246</v>
+      </c>
+      <c r="H62" t="s">
+        <v>247</v>
+      </c>
+      <c r="I62" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1801,8 +3440,23 @@
       <c r="C63" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E63" t="s">
+        <v>112</v>
+      </c>
+      <c r="F63" t="s">
+        <v>246</v>
+      </c>
+      <c r="G63" t="s">
+        <v>246</v>
+      </c>
+      <c r="H63" t="s">
+        <v>247</v>
+      </c>
+      <c r="I63" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1812,8 +3466,23 @@
       <c r="C64" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E64" t="s">
+        <v>114</v>
+      </c>
+      <c r="F64" t="s">
+        <v>246</v>
+      </c>
+      <c r="G64" t="s">
+        <v>246</v>
+      </c>
+      <c r="H64" t="s">
+        <v>247</v>
+      </c>
+      <c r="I64" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1823,8 +3492,23 @@
       <c r="C65" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E65" t="s">
+        <v>116</v>
+      </c>
+      <c r="F65" t="s">
+        <v>246</v>
+      </c>
+      <c r="G65" t="s">
+        <v>246</v>
+      </c>
+      <c r="H65" t="s">
+        <v>247</v>
+      </c>
+      <c r="I65" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1834,8 +3518,23 @@
       <c r="C66" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E66" t="s">
+        <v>118</v>
+      </c>
+      <c r="F66" t="s">
+        <v>246</v>
+      </c>
+      <c r="G66" t="s">
+        <v>246</v>
+      </c>
+      <c r="H66" t="s">
+        <v>247</v>
+      </c>
+      <c r="I66" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1845,8 +3544,23 @@
       <c r="C67" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E67" t="s">
+        <v>120</v>
+      </c>
+      <c r="F67" t="s">
+        <v>246</v>
+      </c>
+      <c r="G67" t="s">
+        <v>246</v>
+      </c>
+      <c r="H67" t="s">
+        <v>247</v>
+      </c>
+      <c r="I67" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1856,8 +3570,23 @@
       <c r="C68" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E68" t="s">
+        <v>122</v>
+      </c>
+      <c r="F68" t="s">
+        <v>246</v>
+      </c>
+      <c r="G68" t="s">
+        <v>246</v>
+      </c>
+      <c r="H68" t="s">
+        <v>247</v>
+      </c>
+      <c r="I68" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1867,8 +3596,23 @@
       <c r="C69" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E69" t="s">
+        <v>124</v>
+      </c>
+      <c r="F69" t="s">
+        <v>246</v>
+      </c>
+      <c r="G69" t="s">
+        <v>246</v>
+      </c>
+      <c r="H69" t="s">
+        <v>247</v>
+      </c>
+      <c r="I69" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1878,8 +3622,23 @@
       <c r="C70" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E70" t="s">
+        <v>126</v>
+      </c>
+      <c r="F70" t="s">
+        <v>246</v>
+      </c>
+      <c r="G70" t="s">
+        <v>246</v>
+      </c>
+      <c r="H70" t="s">
+        <v>247</v>
+      </c>
+      <c r="I70" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1889,8 +3648,23 @@
       <c r="C71" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E71" t="s">
+        <v>130</v>
+      </c>
+      <c r="F71" t="s">
+        <v>246</v>
+      </c>
+      <c r="G71" t="s">
+        <v>246</v>
+      </c>
+      <c r="H71" t="s">
+        <v>247</v>
+      </c>
+      <c r="I71" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1900,8 +3674,23 @@
       <c r="C72" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E72" t="s">
+        <v>132</v>
+      </c>
+      <c r="F72" t="s">
+        <v>246</v>
+      </c>
+      <c r="G72" t="s">
+        <v>246</v>
+      </c>
+      <c r="H72" t="s">
+        <v>247</v>
+      </c>
+      <c r="I72" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1911,8 +3700,23 @@
       <c r="C73" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E73" t="s">
+        <v>134</v>
+      </c>
+      <c r="F73" t="s">
+        <v>246</v>
+      </c>
+      <c r="G73" t="s">
+        <v>246</v>
+      </c>
+      <c r="H73" t="s">
+        <v>247</v>
+      </c>
+      <c r="I73" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1922,8 +3726,23 @@
       <c r="C74" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E74" t="s">
+        <v>135</v>
+      </c>
+      <c r="F74" t="s">
+        <v>246</v>
+      </c>
+      <c r="G74" t="s">
+        <v>246</v>
+      </c>
+      <c r="H74" t="s">
+        <v>247</v>
+      </c>
+      <c r="I74" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1933,8 +3752,23 @@
       <c r="C75" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E75" t="s">
+        <v>137</v>
+      </c>
+      <c r="F75" t="s">
+        <v>246</v>
+      </c>
+      <c r="G75" t="s">
+        <v>246</v>
+      </c>
+      <c r="H75" t="s">
+        <v>247</v>
+      </c>
+      <c r="I75" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1944,8 +3778,23 @@
       <c r="C76" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E76" t="s">
+        <v>138</v>
+      </c>
+      <c r="F76" t="s">
+        <v>246</v>
+      </c>
+      <c r="G76" t="s">
+        <v>246</v>
+      </c>
+      <c r="H76" t="s">
+        <v>247</v>
+      </c>
+      <c r="I76" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1955,16 +3804,46 @@
       <c r="C77" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E77" t="s">
+        <v>140</v>
+      </c>
+      <c r="F77" t="s">
+        <v>246</v>
+      </c>
+      <c r="G77" t="s">
+        <v>246</v>
+      </c>
+      <c r="H77" t="s">
+        <v>247</v>
+      </c>
+      <c r="I77" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E78" t="s">
+        <v>141</v>
+      </c>
+      <c r="F78" t="s">
+        <v>246</v>
+      </c>
+      <c r="G78" t="s">
+        <v>246</v>
+      </c>
+      <c r="H78" t="s">
+        <v>247</v>
+      </c>
+      <c r="I78" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1974,8 +3853,23 @@
       <c r="C79" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E79" t="s">
+        <v>142</v>
+      </c>
+      <c r="F79" t="s">
+        <v>246</v>
+      </c>
+      <c r="G79" t="s">
+        <v>246</v>
+      </c>
+      <c r="H79" t="s">
+        <v>247</v>
+      </c>
+      <c r="I79" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1985,8 +3879,23 @@
       <c r="C80" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E80" t="s">
+        <v>144</v>
+      </c>
+      <c r="F80" t="s">
+        <v>246</v>
+      </c>
+      <c r="G80" t="s">
+        <v>246</v>
+      </c>
+      <c r="H80" t="s">
+        <v>247</v>
+      </c>
+      <c r="I80" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1996,8 +3905,23 @@
       <c r="C81" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E81" t="s">
+        <v>147</v>
+      </c>
+      <c r="F81" t="s">
+        <v>246</v>
+      </c>
+      <c r="G81" t="s">
+        <v>246</v>
+      </c>
+      <c r="H81" t="s">
+        <v>247</v>
+      </c>
+      <c r="I81" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2007,8 +3931,23 @@
       <c r="C82" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E82" t="s">
+        <v>149</v>
+      </c>
+      <c r="F82" t="s">
+        <v>246</v>
+      </c>
+      <c r="G82" t="s">
+        <v>246</v>
+      </c>
+      <c r="H82" t="s">
+        <v>247</v>
+      </c>
+      <c r="I82" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2018,8 +3957,23 @@
       <c r="C83" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E83" t="s">
+        <v>151</v>
+      </c>
+      <c r="F83" t="s">
+        <v>246</v>
+      </c>
+      <c r="G83" t="s">
+        <v>246</v>
+      </c>
+      <c r="H83" t="s">
+        <v>247</v>
+      </c>
+      <c r="I83" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2029,8 +3983,23 @@
       <c r="C84" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E84" t="s">
+        <v>153</v>
+      </c>
+      <c r="F84" t="s">
+        <v>246</v>
+      </c>
+      <c r="G84" t="s">
+        <v>246</v>
+      </c>
+      <c r="H84" t="s">
+        <v>247</v>
+      </c>
+      <c r="I84" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2040,8 +4009,23 @@
       <c r="C85" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E85" t="s">
+        <v>155</v>
+      </c>
+      <c r="F85" t="s">
+        <v>246</v>
+      </c>
+      <c r="G85" t="s">
+        <v>246</v>
+      </c>
+      <c r="H85" t="s">
+        <v>247</v>
+      </c>
+      <c r="I85" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2051,8 +4035,23 @@
       <c r="C86" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E86" t="s">
+        <v>156</v>
+      </c>
+      <c r="F86" t="s">
+        <v>246</v>
+      </c>
+      <c r="G86" t="s">
+        <v>246</v>
+      </c>
+      <c r="H86" t="s">
+        <v>247</v>
+      </c>
+      <c r="I86" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2062,8 +4061,23 @@
       <c r="C87" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E87" t="s">
+        <v>158</v>
+      </c>
+      <c r="F87" t="s">
+        <v>246</v>
+      </c>
+      <c r="G87" t="s">
+        <v>246</v>
+      </c>
+      <c r="H87" t="s">
+        <v>247</v>
+      </c>
+      <c r="I87" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2073,8 +4087,23 @@
       <c r="C88" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E88" t="s">
+        <v>160</v>
+      </c>
+      <c r="F88" t="s">
+        <v>246</v>
+      </c>
+      <c r="G88" t="s">
+        <v>246</v>
+      </c>
+      <c r="H88" t="s">
+        <v>247</v>
+      </c>
+      <c r="I88" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2084,8 +4113,23 @@
       <c r="C89" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E89" t="s">
+        <v>162</v>
+      </c>
+      <c r="F89" t="s">
+        <v>246</v>
+      </c>
+      <c r="G89" t="s">
+        <v>246</v>
+      </c>
+      <c r="H89" t="s">
+        <v>247</v>
+      </c>
+      <c r="I89" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2095,8 +4139,23 @@
       <c r="C90" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E90" t="s">
+        <v>164</v>
+      </c>
+      <c r="F90" t="s">
+        <v>246</v>
+      </c>
+      <c r="G90" t="s">
+        <v>246</v>
+      </c>
+      <c r="H90" t="s">
+        <v>247</v>
+      </c>
+      <c r="I90" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2106,8 +4165,23 @@
       <c r="C91" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E91" t="s">
+        <v>168</v>
+      </c>
+      <c r="F91" t="s">
+        <v>246</v>
+      </c>
+      <c r="G91" t="s">
+        <v>246</v>
+      </c>
+      <c r="H91" t="s">
+        <v>247</v>
+      </c>
+      <c r="I91" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2117,8 +4191,23 @@
       <c r="C92" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E92" t="s">
+        <v>170</v>
+      </c>
+      <c r="F92" t="s">
+        <v>246</v>
+      </c>
+      <c r="G92" t="s">
+        <v>246</v>
+      </c>
+      <c r="H92" t="s">
+        <v>247</v>
+      </c>
+      <c r="I92" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2128,8 +4217,23 @@
       <c r="C93" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E93" t="s">
+        <v>172</v>
+      </c>
+      <c r="F93" t="s">
+        <v>246</v>
+      </c>
+      <c r="G93" t="s">
+        <v>246</v>
+      </c>
+      <c r="H93" t="s">
+        <v>247</v>
+      </c>
+      <c r="I93" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2139,8 +4243,23 @@
       <c r="C94" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E94" t="s">
+        <v>174</v>
+      </c>
+      <c r="F94" t="s">
+        <v>246</v>
+      </c>
+      <c r="G94" t="s">
+        <v>246</v>
+      </c>
+      <c r="H94" t="s">
+        <v>247</v>
+      </c>
+      <c r="I94" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2150,8 +4269,23 @@
       <c r="C95" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E95" t="s">
+        <v>176</v>
+      </c>
+      <c r="F95" t="s">
+        <v>246</v>
+      </c>
+      <c r="G95" t="s">
+        <v>246</v>
+      </c>
+      <c r="H95" t="s">
+        <v>247</v>
+      </c>
+      <c r="I95" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2161,8 +4295,23 @@
       <c r="C96" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E96" t="s">
+        <v>178</v>
+      </c>
+      <c r="F96" t="s">
+        <v>246</v>
+      </c>
+      <c r="G96" t="s">
+        <v>246</v>
+      </c>
+      <c r="H96" t="s">
+        <v>247</v>
+      </c>
+      <c r="I96" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2172,8 +4321,23 @@
       <c r="C97" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E97" t="s">
+        <v>180</v>
+      </c>
+      <c r="F97" t="s">
+        <v>246</v>
+      </c>
+      <c r="G97" t="s">
+        <v>246</v>
+      </c>
+      <c r="H97" t="s">
+        <v>247</v>
+      </c>
+      <c r="I97" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2183,8 +4347,23 @@
       <c r="C98" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E98" t="s">
+        <v>182</v>
+      </c>
+      <c r="F98" t="s">
+        <v>246</v>
+      </c>
+      <c r="G98" t="s">
+        <v>246</v>
+      </c>
+      <c r="H98" t="s">
+        <v>247</v>
+      </c>
+      <c r="I98" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2194,8 +4373,23 @@
       <c r="C99" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E99" t="s">
+        <v>183</v>
+      </c>
+      <c r="F99" t="s">
+        <v>246</v>
+      </c>
+      <c r="G99" t="s">
+        <v>246</v>
+      </c>
+      <c r="H99" t="s">
+        <v>247</v>
+      </c>
+      <c r="I99" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2205,8 +4399,23 @@
       <c r="C100" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E100" t="s">
+        <v>185</v>
+      </c>
+      <c r="F100" t="s">
+        <v>246</v>
+      </c>
+      <c r="G100" t="s">
+        <v>246</v>
+      </c>
+      <c r="H100" t="s">
+        <v>247</v>
+      </c>
+      <c r="I100" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2215,6 +4424,21 @@
       </c>
       <c r="C101" t="s">
         <v>8</v>
+      </c>
+      <c r="E101" t="s">
+        <v>7</v>
+      </c>
+      <c r="F101" t="s">
+        <v>246</v>
+      </c>
+      <c r="G101" t="s">
+        <v>246</v>
+      </c>
+      <c r="H101" t="s">
+        <v>247</v>
+      </c>
+      <c r="I101" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -2229,10 +4453,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:BK58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2240,475 +4464,1325 @@
     <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>187</v>
       </c>
       <c r="B1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>249</v>
+      </c>
+      <c r="H1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I1" t="s">
+        <v>251</v>
+      </c>
+      <c r="J1" t="s">
+        <v>252</v>
+      </c>
+      <c r="K1" t="s">
+        <v>253</v>
+      </c>
+      <c r="L1" t="s">
+        <v>254</v>
+      </c>
+      <c r="M1" t="s">
+        <v>255</v>
+      </c>
+      <c r="N1" t="s">
+        <v>256</v>
+      </c>
+      <c r="O1" t="s">
+        <v>257</v>
+      </c>
+      <c r="P1" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>259</v>
+      </c>
+      <c r="R1" t="s">
+        <v>260</v>
+      </c>
+      <c r="S1" t="s">
+        <v>261</v>
+      </c>
+      <c r="T1" t="s">
+        <v>262</v>
+      </c>
+      <c r="U1" t="s">
+        <v>263</v>
+      </c>
+      <c r="V1" t="s">
+        <v>264</v>
+      </c>
+      <c r="W1" t="s">
+        <v>265</v>
+      </c>
+      <c r="X1" t="s">
+        <v>266</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>268</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>271</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>272</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>273</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>274</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>275</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>276</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>277</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>278</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>279</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>280</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>281</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>231</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>232</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>234</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>235</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>236</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>237</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>238</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>282</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>240</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>241</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>242</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>243</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>244</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E3" t="s">
+        <v>248</v>
+      </c>
+      <c r="F3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" t="s">
+        <v>248</v>
+      </c>
+      <c r="F5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" t="s">
+        <v>246</v>
+      </c>
+      <c r="E6" t="s">
+        <v>248</v>
+      </c>
+      <c r="F6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E7" t="s">
+        <v>248</v>
+      </c>
+      <c r="F7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="8" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>246</v>
+      </c>
+      <c r="D8" t="s">
+        <v>246</v>
+      </c>
+      <c r="E8" t="s">
+        <v>248</v>
+      </c>
+      <c r="F8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D9" t="s">
+        <v>246</v>
+      </c>
+      <c r="E9" t="s">
+        <v>248</v>
+      </c>
+      <c r="F9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>246</v>
+      </c>
+      <c r="D10" t="s">
+        <v>246</v>
+      </c>
+      <c r="E10" t="s">
+        <v>248</v>
+      </c>
+      <c r="F10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D11" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" t="s">
+        <v>248</v>
+      </c>
+      <c r="F11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>246</v>
+      </c>
+      <c r="D12" t="s">
+        <v>246</v>
+      </c>
+      <c r="E12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>246</v>
+      </c>
+      <c r="D13" t="s">
+        <v>246</v>
+      </c>
+      <c r="E13" t="s">
+        <v>248</v>
+      </c>
+      <c r="F13" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>246</v>
+      </c>
+      <c r="D14" t="s">
+        <v>246</v>
+      </c>
+      <c r="E14" t="s">
+        <v>248</v>
+      </c>
+      <c r="F14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>246</v>
+      </c>
+      <c r="D15" t="s">
+        <v>246</v>
+      </c>
+      <c r="E15" t="s">
+        <v>248</v>
+      </c>
+      <c r="F15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>246</v>
+      </c>
+      <c r="D16" t="s">
+        <v>246</v>
+      </c>
+      <c r="E16" t="s">
+        <v>248</v>
+      </c>
+      <c r="F16" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>246</v>
+      </c>
+      <c r="D17" t="s">
+        <v>246</v>
+      </c>
+      <c r="E17" t="s">
+        <v>248</v>
+      </c>
+      <c r="F17" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>246</v>
+      </c>
+      <c r="D18" t="s">
+        <v>246</v>
+      </c>
+      <c r="E18" t="s">
+        <v>248</v>
+      </c>
+      <c r="F18" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>246</v>
+      </c>
+      <c r="D19" t="s">
+        <v>246</v>
+      </c>
+      <c r="E19" t="s">
+        <v>248</v>
+      </c>
+      <c r="F19" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>246</v>
+      </c>
+      <c r="D20" t="s">
+        <v>246</v>
+      </c>
+      <c r="E20" t="s">
+        <v>248</v>
+      </c>
+      <c r="F20" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>246</v>
+      </c>
+      <c r="D21" t="s">
+        <v>246</v>
+      </c>
+      <c r="E21" t="s">
+        <v>248</v>
+      </c>
+      <c r="F21" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>246</v>
+      </c>
+      <c r="D22" t="s">
+        <v>246</v>
+      </c>
+      <c r="E22" t="s">
+        <v>248</v>
+      </c>
+      <c r="F22" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>246</v>
+      </c>
+      <c r="D23" t="s">
+        <v>246</v>
+      </c>
+      <c r="E23" t="s">
+        <v>248</v>
+      </c>
+      <c r="F23" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>246</v>
+      </c>
+      <c r="D24" t="s">
+        <v>246</v>
+      </c>
+      <c r="E24" t="s">
+        <v>248</v>
+      </c>
+      <c r="F24" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>246</v>
+      </c>
+      <c r="D25" t="s">
+        <v>246</v>
+      </c>
+      <c r="E25" t="s">
+        <v>248</v>
+      </c>
+      <c r="F25" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D26" t="s">
+        <v>246</v>
+      </c>
+      <c r="E26" t="s">
+        <v>248</v>
+      </c>
+      <c r="F26" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>246</v>
+      </c>
+      <c r="D27" t="s">
+        <v>246</v>
+      </c>
+      <c r="E27" t="s">
+        <v>248</v>
+      </c>
+      <c r="F27" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>246</v>
+      </c>
+      <c r="D28" t="s">
+        <v>246</v>
+      </c>
+      <c r="E28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F28" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>246</v>
+      </c>
+      <c r="D29" t="s">
+        <v>246</v>
+      </c>
+      <c r="E29" t="s">
+        <v>248</v>
+      </c>
+      <c r="F29" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>246</v>
+      </c>
+      <c r="D30" t="s">
+        <v>246</v>
+      </c>
+      <c r="E30" t="s">
+        <v>248</v>
+      </c>
+      <c r="F30" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>246</v>
+      </c>
+      <c r="D31" t="s">
+        <v>246</v>
+      </c>
+      <c r="E31" t="s">
+        <v>248</v>
+      </c>
+      <c r="F31" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>246</v>
+      </c>
+      <c r="D32" t="s">
+        <v>246</v>
+      </c>
+      <c r="E32" t="s">
+        <v>248</v>
+      </c>
+      <c r="F32" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>246</v>
+      </c>
+      <c r="D33" t="s">
+        <v>246</v>
+      </c>
+      <c r="E33" t="s">
+        <v>248</v>
+      </c>
+      <c r="F33" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>221</v>
       </c>
-      <c r="C34" s="1">
-        <v>43453</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>246</v>
+      </c>
+      <c r="D34" t="s">
+        <v>246</v>
+      </c>
+      <c r="E34" t="s">
+        <v>248</v>
+      </c>
+      <c r="F34" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>246</v>
+      </c>
+      <c r="D35" t="s">
+        <v>246</v>
+      </c>
+      <c r="E35" t="s">
+        <v>248</v>
+      </c>
+      <c r="F35" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>246</v>
+      </c>
+      <c r="D36" t="s">
+        <v>246</v>
+      </c>
+      <c r="E36" t="s">
+        <v>248</v>
+      </c>
+      <c r="F36" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>246</v>
+      </c>
+      <c r="D37" t="s">
+        <v>246</v>
+      </c>
+      <c r="E37" t="s">
+        <v>248</v>
+      </c>
+      <c r="F37" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>246</v>
+      </c>
+      <c r="D38" t="s">
+        <v>246</v>
+      </c>
+      <c r="E38" t="s">
+        <v>248</v>
+      </c>
+      <c r="F38" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>246</v>
+      </c>
+      <c r="D39" t="s">
+        <v>246</v>
+      </c>
+      <c r="E39" t="s">
+        <v>248</v>
+      </c>
+      <c r="F39" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>246</v>
+      </c>
+      <c r="D40" t="s">
+        <v>246</v>
+      </c>
+      <c r="E40" t="s">
+        <v>248</v>
+      </c>
+      <c r="F40" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>246</v>
+      </c>
+      <c r="D41" t="s">
+        <v>246</v>
+      </c>
+      <c r="E41" t="s">
+        <v>248</v>
+      </c>
+      <c r="F41" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>246</v>
+      </c>
+      <c r="D42" t="s">
+        <v>246</v>
+      </c>
+      <c r="E42" t="s">
+        <v>248</v>
+      </c>
+      <c r="F42" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>246</v>
+      </c>
+      <c r="D43" t="s">
+        <v>246</v>
+      </c>
+      <c r="E43" t="s">
+        <v>248</v>
+      </c>
+      <c r="F43" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>246</v>
+      </c>
+      <c r="D44" t="s">
+        <v>246</v>
+      </c>
+      <c r="E44" t="s">
+        <v>248</v>
+      </c>
+      <c r="F44" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>246</v>
+      </c>
+      <c r="D45" t="s">
+        <v>246</v>
+      </c>
+      <c r="E45" t="s">
+        <v>248</v>
+      </c>
+      <c r="F45" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>246</v>
+      </c>
+      <c r="D46" t="s">
+        <v>246</v>
+      </c>
+      <c r="E46" t="s">
+        <v>248</v>
+      </c>
+      <c r="F46" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>246</v>
+      </c>
+      <c r="D47" t="s">
+        <v>246</v>
+      </c>
+      <c r="E47" t="s">
+        <v>248</v>
+      </c>
+      <c r="F47" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>246</v>
+      </c>
+      <c r="D48" t="s">
+        <v>246</v>
+      </c>
+      <c r="E48" t="s">
+        <v>248</v>
+      </c>
+      <c r="F48" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>246</v>
+      </c>
+      <c r="D49" t="s">
+        <v>246</v>
+      </c>
+      <c r="E49" t="s">
+        <v>248</v>
+      </c>
+      <c r="F49" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>246</v>
+      </c>
+      <c r="D50" t="s">
+        <v>246</v>
+      </c>
+      <c r="E50" t="s">
+        <v>248</v>
+      </c>
+      <c r="F50" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>246</v>
+      </c>
+      <c r="D51" t="s">
+        <v>246</v>
+      </c>
+      <c r="E51" t="s">
+        <v>248</v>
+      </c>
+      <c r="F51" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>239</v>
       </c>
-      <c r="C52" s="1">
-        <v>43425</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>246</v>
+      </c>
+      <c r="D52" t="s">
+        <v>246</v>
+      </c>
+      <c r="E52" t="s">
+        <v>248</v>
+      </c>
+      <c r="F52" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>246</v>
+      </c>
+      <c r="D53" t="s">
+        <v>246</v>
+      </c>
+      <c r="E53" t="s">
+        <v>248</v>
+      </c>
+      <c r="F53" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>246</v>
+      </c>
+      <c r="D54" t="s">
+        <v>246</v>
+      </c>
+      <c r="E54" t="s">
+        <v>248</v>
+      </c>
+      <c r="F54" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>246</v>
+      </c>
+      <c r="D55" t="s">
+        <v>246</v>
+      </c>
+      <c r="E55" t="s">
+        <v>248</v>
+      </c>
+      <c r="F55" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>246</v>
+      </c>
+      <c r="D56" t="s">
+        <v>246</v>
+      </c>
+      <c r="E56" t="s">
+        <v>248</v>
+      </c>
+      <c r="F56" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>246</v>
+      </c>
+      <c r="D57" t="s">
+        <v>246</v>
+      </c>
+      <c r="E57" t="s">
+        <v>248</v>
+      </c>
+      <c r="F57" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>245</v>
+      </c>
+      <c r="C58" t="s">
+        <v>246</v>
+      </c>
+      <c r="D58" t="s">
+        <v>246</v>
+      </c>
+      <c r="E58" t="s">
+        <v>248</v>
+      </c>
+      <c r="F58" t="s">
         <v>245</v>
       </c>
     </row>

</xml_diff>